<commit_message>
Optimized Project with POM design Pattern for Login, Register and Search Page. Added Screenshot on Failure Method
</commit_message>
<xml_diff>
--- a/AutomationPracticeApp/src/main/java/org/project/qa/testData/TutorialsNinjaTestData.xlsx
+++ b/AutomationPracticeApp/src/main/java/org/project/qa/testData/TutorialsNinjaTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hariv\OneDrive\Documents\Testing Projects\AutomationPracticeApp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hariv\OneDrive\Documents\Testing Projects\AutomationPracticeApp\src\main\java\org\project\qa\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D8B8CA8-88D6-4C1A-BC58-727B4371246C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE964742-8552-47CE-A150-7398341F6879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="3240" windowWidth="17280" windowHeight="8880" xr2:uid="{D522A685-CB54-47DE-8A33-224A9D2969C8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D522A685-CB54-47DE-8A33-224A9D2969C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="4">
   <si>
     <t>Email</t>
   </si>
@@ -37,12 +37,6 @@
   </si>
   <si>
     <t>Testing0@</t>
-  </si>
-  <si>
-    <t>tpreactice@gmail.com</t>
-  </si>
-  <si>
-    <t>tepas@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -84,10 +78,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,7 +398,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -423,34 +416,34 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>12345</v>
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>324542</v>
+      <c r="B4" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>